<commit_message>
add presentation with file for paper
</commit_message>
<xml_diff>
--- a/Biomod_variable_importance_summary.xlsx
+++ b/Biomod_variable_importance_summary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="HGAM_tables" sheetId="1" state="visible" r:id="rId2"/>
@@ -868,7 +868,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1003,10 +1003,6 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1152,11 +1148,11 @@
   </sheetPr>
   <dimension ref="A1:AK79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AG74" activeCellId="0" sqref="AG74"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AG74" activeCellId="1" sqref="S19:S24 AG74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.52"/>
@@ -1166,7 +1162,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="13.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="13.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="13.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="11.11"/>
@@ -2365,7 +2361,7 @@
       <c r="R31" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="V31" s="34" t="s">
+      <c r="V31" s="1" t="s">
         <v>113</v>
       </c>
       <c r="W31" s="0" t="n">
@@ -2458,7 +2454,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V34" s="34" t="s">
+      <c r="V34" s="1" t="s">
         <v>117</v>
       </c>
       <c r="W34" s="0" t="n">
@@ -2508,7 +2504,7 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V36" s="35" t="s">
+      <c r="V36" s="34" t="s">
         <v>119</v>
       </c>
       <c r="W36" s="0" t="n">
@@ -2533,14 +2529,14 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N37" s="36"/>
-      <c r="O37" s="36"/>
-      <c r="P37" s="36"/>
-      <c r="Q37" s="36"/>
-      <c r="R37" s="36"/>
-      <c r="S37" s="36"/>
-      <c r="T37" s="36"/>
-      <c r="U37" s="36"/>
+      <c r="N37" s="35"/>
+      <c r="O37" s="35"/>
+      <c r="P37" s="35"/>
+      <c r="Q37" s="35"/>
+      <c r="R37" s="35"/>
+      <c r="S37" s="35"/>
+      <c r="T37" s="35"/>
+      <c r="U37" s="35"/>
       <c r="V37" s="0" t="s">
         <v>120</v>
       </c>
@@ -2660,7 +2656,7 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V44" s="34" t="s">
+      <c r="V44" s="1" t="s">
         <v>113</v>
       </c>
       <c r="W44" s="0" t="n">
@@ -2735,7 +2731,7 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V47" s="34" t="s">
+      <c r="V47" s="1" t="s">
         <v>117</v>
       </c>
       <c r="W47" s="0" t="n">
@@ -2785,7 +2781,7 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V49" s="35" t="s">
+      <c r="V49" s="34" t="s">
         <v>119</v>
       </c>
       <c r="W49" s="0" t="n">
@@ -2865,17 +2861,17 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AC55" s="37"/>
-      <c r="AD55" s="38" t="s">
+      <c r="AC55" s="36"/>
+      <c r="AD55" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="AE55" s="39"/>
-      <c r="AF55" s="39"/>
-      <c r="AG55" s="38" t="s">
+      <c r="AE55" s="38"/>
+      <c r="AF55" s="38"/>
+      <c r="AG55" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="AH55" s="39"/>
-      <c r="AI55" s="40"/>
+      <c r="AH55" s="38"/>
+      <c r="AI55" s="39"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W56" s="0" t="s">
@@ -2887,23 +2883,23 @@
       <c r="Y56" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="AC56" s="41"/>
-      <c r="AD56" s="42" t="s">
+      <c r="AC56" s="40"/>
+      <c r="AD56" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="AE56" s="42" t="s">
+      <c r="AE56" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="AF56" s="42" t="s">
+      <c r="AF56" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="AG56" s="42" t="s">
+      <c r="AG56" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="AH56" s="42" t="s">
+      <c r="AH56" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="AI56" s="43" t="s">
+      <c r="AI56" s="42" t="s">
         <v>107</v>
       </c>
       <c r="AJ56" s="2"/>
@@ -2937,13 +2933,13 @@
       <c r="AF57" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="AG57" s="44" t="n">
+      <c r="AG57" s="43" t="n">
         <v>0.946</v>
       </c>
-      <c r="AH57" s="44" t="n">
+      <c r="AH57" s="43" t="n">
         <v>0.344</v>
       </c>
-      <c r="AI57" s="45" t="s">
+      <c r="AI57" s="44" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2975,13 +2971,13 @@
       <c r="AF58" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="AG58" s="44" t="n">
+      <c r="AG58" s="43" t="n">
         <v>1.118</v>
       </c>
-      <c r="AH58" s="44" t="n">
+      <c r="AH58" s="43" t="n">
         <v>0.344</v>
       </c>
-      <c r="AI58" s="45" t="s">
+      <c r="AI58" s="44" t="s">
         <v>130</v>
       </c>
     </row>
@@ -3013,13 +3009,13 @@
       <c r="AF59" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="AG59" s="44" t="n">
+      <c r="AG59" s="43" t="n">
         <v>0.731</v>
       </c>
-      <c r="AH59" s="44" t="n">
+      <c r="AH59" s="43" t="n">
         <v>0.344</v>
       </c>
-      <c r="AI59" s="45" t="s">
+      <c r="AI59" s="44" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3051,13 +3047,13 @@
       <c r="AF60" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="AG60" s="44" t="n">
+      <c r="AG60" s="43" t="n">
         <v>0.903</v>
       </c>
-      <c r="AH60" s="44" t="n">
+      <c r="AH60" s="43" t="n">
         <v>0.43</v>
       </c>
-      <c r="AI60" s="45" t="s">
+      <c r="AI60" s="44" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3089,13 +3085,13 @@
       <c r="AF61" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="AG61" s="44" t="n">
+      <c r="AG61" s="43" t="n">
         <v>0.774</v>
       </c>
-      <c r="AH61" s="44" t="n">
+      <c r="AH61" s="43" t="n">
         <v>0.387</v>
       </c>
-      <c r="AI61" s="45" t="s">
+      <c r="AI61" s="44" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3127,13 +3123,13 @@
       <c r="AF62" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="AG62" s="44" t="n">
+      <c r="AG62" s="43" t="n">
         <v>0.172</v>
       </c>
-      <c r="AH62" s="44" t="n">
+      <c r="AH62" s="43" t="n">
         <v>0.344</v>
       </c>
-      <c r="AI62" s="45" t="s">
+      <c r="AI62" s="44" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3165,13 +3161,13 @@
       <c r="AF63" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="AG63" s="44" t="n">
+      <c r="AG63" s="43" t="n">
         <v>1.763</v>
       </c>
-      <c r="AH63" s="44" t="n">
+      <c r="AH63" s="43" t="n">
         <v>0.344</v>
       </c>
-      <c r="AI63" s="45" t="s">
+      <c r="AI63" s="44" t="s">
         <v>128</v>
       </c>
     </row>
@@ -3203,13 +3199,13 @@
       <c r="AF64" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="AG64" s="44" t="n">
+      <c r="AG64" s="43" t="n">
         <v>1.978</v>
       </c>
-      <c r="AH64" s="44" t="n">
+      <c r="AH64" s="43" t="n">
         <v>0.387</v>
       </c>
-      <c r="AI64" s="45" t="s">
+      <c r="AI64" s="44" t="s">
         <v>128</v>
       </c>
     </row>
@@ -3241,13 +3237,13 @@
       <c r="AF65" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="AG65" s="44" t="n">
+      <c r="AG65" s="43" t="n">
         <v>1.892</v>
       </c>
-      <c r="AH65" s="44" t="n">
+      <c r="AH65" s="43" t="n">
         <v>0.344</v>
       </c>
-      <c r="AI65" s="45" t="s">
+      <c r="AI65" s="44" t="s">
         <v>128</v>
       </c>
     </row>
@@ -3270,13 +3266,13 @@
       <c r="AC66" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="AD66" s="46" t="n">
+      <c r="AD66" s="45" t="n">
         <v>1.204</v>
       </c>
-      <c r="AE66" s="46" t="n">
+      <c r="AE66" s="45" t="n">
         <v>0.215</v>
       </c>
-      <c r="AF66" s="46" t="s">
+      <c r="AF66" s="45" t="s">
         <v>128</v>
       </c>
       <c r="AG66" s="12" t="n">
@@ -3295,13 +3291,13 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="W69" s="47" t="s">
+      <c r="W69" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="X69" s="47" t="s">
+      <c r="X69" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="Y69" s="47" t="s">
+      <c r="Y69" s="46" t="s">
         <v>107</v>
       </c>
       <c r="Z69" s="0" t="s">
@@ -3321,7 +3317,7 @@
       <c r="X70" s="7" t="n">
         <v>0.344</v>
       </c>
-      <c r="Y70" s="48" t="n">
+      <c r="Y70" s="47" t="n">
         <v>0.0093</v>
       </c>
       <c r="Z70" s="7" t="s">
@@ -3341,7 +3337,7 @@
       <c r="X71" s="7" t="n">
         <v>0.344</v>
       </c>
-      <c r="Y71" s="48" t="n">
+      <c r="Y71" s="47" t="n">
         <v>0.0036</v>
       </c>
       <c r="Z71" s="7" t="s">
@@ -3361,7 +3357,7 @@
       <c r="X72" s="7" t="n">
         <v>0.344</v>
       </c>
-      <c r="Y72" s="48" t="n">
+      <c r="Y72" s="47" t="n">
         <v>0.0491</v>
       </c>
       <c r="Z72" s="7" t="s">
@@ -3381,7 +3377,7 @@
       <c r="X73" s="7" t="n">
         <v>0.43</v>
       </c>
-      <c r="Y73" s="48" t="n">
+      <c r="Y73" s="47" t="n">
         <v>0.037</v>
       </c>
       <c r="Z73" s="7" t="s">
@@ -3401,7 +3397,7 @@
       <c r="X74" s="7" t="n">
         <v>0.387</v>
       </c>
-      <c r="Y74" s="48" t="n">
+      <c r="Y74" s="47" t="n">
         <v>0.07</v>
       </c>
       <c r="Z74" s="7" t="s">
@@ -3421,7 +3417,7 @@
       <c r="X75" s="7" t="n">
         <v>0.344</v>
       </c>
-      <c r="Y75" s="48" t="n">
+      <c r="Y75" s="47" t="n">
         <v>0.645</v>
       </c>
       <c r="Z75" s="7" t="s">
@@ -3441,7 +3437,7 @@
       <c r="X76" s="7" t="n">
         <v>0.344</v>
       </c>
-      <c r="Y76" s="48" t="n">
+      <c r="Y76" s="47" t="n">
         <v>1.65E-005</v>
       </c>
       <c r="Z76" s="7" t="s">
@@ -3461,7 +3457,7 @@
       <c r="X77" s="7" t="n">
         <v>0.387</v>
       </c>
-      <c r="Y77" s="48" t="n">
+      <c r="Y77" s="47" t="n">
         <v>1.6E-005</v>
       </c>
       <c r="Z77" s="7" t="s">
@@ -3481,7 +3477,7 @@
       <c r="X78" s="7" t="n">
         <v>0.344</v>
       </c>
-      <c r="Y78" s="48" t="n">
+      <c r="Y78" s="47" t="n">
         <v>1E-006</v>
       </c>
       <c r="Z78" s="7" t="s">
@@ -3501,7 +3497,7 @@
       <c r="X79" s="7" t="n">
         <v>0.344</v>
       </c>
-      <c r="Y79" s="48" t="n">
+      <c r="Y79" s="47" t="n">
         <v>8E-006</v>
       </c>
       <c r="Z79" s="7" t="s">
@@ -3530,10 +3526,10 @@
   <dimension ref="A1:P40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F48" activeCellId="0" sqref="F48"/>
+      <selection pane="topLeft" activeCell="F48" activeCellId="1" sqref="S19:S24 F48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="41.44"/>
@@ -3637,22 +3633,22 @@
       <c r="A3" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="B3" s="49" t="n">
+      <c r="B3" s="48" t="n">
         <v>0.33</v>
       </c>
-      <c r="C3" s="49" t="n">
+      <c r="C3" s="48" t="n">
         <v>0.29</v>
       </c>
-      <c r="D3" s="49" t="n">
+      <c r="D3" s="48" t="n">
         <v>10751</v>
       </c>
-      <c r="E3" s="49" t="n">
+      <c r="E3" s="48" t="n">
         <v>4424</v>
       </c>
-      <c r="F3" s="49" t="n">
+      <c r="F3" s="48" t="n">
         <v>175</v>
       </c>
-      <c r="G3" s="49" t="n">
+      <c r="G3" s="48" t="n">
         <v>131</v>
       </c>
       <c r="H3" s="0" t="n">
@@ -3670,13 +3666,13 @@
       <c r="M3" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="N3" s="49" t="n">
+      <c r="N3" s="48" t="n">
         <v>0.79585573923861</v>
       </c>
       <c r="O3" s="0" t="n">
         <v>0.879550383717047</v>
       </c>
-      <c r="P3" s="49" t="n">
+      <c r="P3" s="48" t="n">
         <v>0.869013084556499</v>
       </c>
     </row>
@@ -3728,16 +3724,16 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="48" t="s">
         <v>159</v>
       </c>
-      <c r="B5" s="50" t="n">
+      <c r="B5" s="49" t="n">
         <v>0.32</v>
       </c>
-      <c r="C5" s="50" t="n">
+      <c r="C5" s="49" t="n">
         <v>0.25</v>
       </c>
-      <c r="D5" s="50" t="n">
+      <c r="D5" s="49" t="n">
         <v>10819</v>
       </c>
       <c r="E5" s="0" t="n">
@@ -3767,10 +3763,10 @@
       <c r="N5" s="0" t="n">
         <v>0.794071331934039</v>
       </c>
-      <c r="O5" s="49" t="n">
+      <c r="O5" s="48" t="n">
         <v>0.879802719386047</v>
       </c>
-      <c r="P5" s="50" t="n">
+      <c r="P5" s="49" t="n">
         <v>0.868560120533409</v>
       </c>
     </row>
@@ -3787,7 +3783,7 @@
       <c r="D6" s="0" t="n">
         <v>10846</v>
       </c>
-      <c r="E6" s="50" t="n">
+      <c r="E6" s="49" t="n">
         <v>4482</v>
       </c>
       <c r="F6" s="0" t="n">
@@ -3811,10 +3807,10 @@
       <c r="M6" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="N6" s="50" t="n">
+      <c r="N6" s="49" t="n">
         <v>0.795535150807621</v>
       </c>
-      <c r="O6" s="50" t="n">
+      <c r="O6" s="49" t="n">
         <v>0.879675508842174</v>
       </c>
       <c r="P6" s="0" t="n">
@@ -3825,7 +3821,7 @@
       <c r="A7" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="B7" s="50" t="n">
+      <c r="B7" s="49" t="n">
         <v>0.32</v>
       </c>
       <c r="C7" s="0" t="n">
@@ -3837,10 +3833,10 @@
       <c r="E7" s="0" t="n">
         <v>4510</v>
       </c>
-      <c r="F7" s="50" t="n">
+      <c r="F7" s="49" t="n">
         <v>118</v>
       </c>
-      <c r="G7" s="50" t="n">
+      <c r="G7" s="49" t="n">
         <v>86</v>
       </c>
       <c r="H7" s="0" t="n">
@@ -3955,7 +3951,7 @@
       <c r="N11" s="0" t="n">
         <v>0.908215733072771</v>
       </c>
-      <c r="O11" s="49" t="n">
+      <c r="O11" s="48" t="n">
         <v>0.904921005564383</v>
       </c>
       <c r="P11" s="0" t="n">
@@ -3966,22 +3962,22 @@
       <c r="A12" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="49" t="n">
+      <c r="B12" s="48" t="n">
         <v>0.4</v>
       </c>
-      <c r="C12" s="49" t="n">
+      <c r="C12" s="48" t="n">
         <v>0.3</v>
       </c>
-      <c r="D12" s="49" t="n">
+      <c r="D12" s="48" t="n">
         <v>9358</v>
       </c>
-      <c r="E12" s="49" t="n">
+      <c r="E12" s="48" t="n">
         <v>7048</v>
       </c>
-      <c r="F12" s="49" t="n">
+      <c r="F12" s="48" t="n">
         <v>186</v>
       </c>
-      <c r="G12" s="49" t="n">
+      <c r="G12" s="48" t="n">
         <v>114</v>
       </c>
       <c r="H12" s="0" t="n">
@@ -3999,13 +3995,13 @@
       <c r="M12" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="N12" s="49" t="n">
+      <c r="N12" s="48" t="n">
         <v>0.917140156932561</v>
       </c>
       <c r="O12" s="0" t="n">
         <v>0.90316722972973</v>
       </c>
-      <c r="P12" s="49" t="n">
+      <c r="P12" s="48" t="n">
         <v>0.864866820422385</v>
       </c>
     </row>
@@ -4063,7 +4059,7 @@
       <c r="B14" s="0" t="n">
         <v>0.38</v>
       </c>
-      <c r="C14" s="50" t="n">
+      <c r="C14" s="49" t="n">
         <v>0.27</v>
       </c>
       <c r="D14" s="0" t="n">
@@ -4099,12 +4095,12 @@
       <c r="O14" s="0" t="n">
         <v>0.903174682034975</v>
       </c>
-      <c r="P14" s="50" t="n">
+      <c r="P14" s="49" t="n">
         <v>0.860821688599465</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="49" t="s">
+      <c r="A15" s="48" t="s">
         <v>166</v>
       </c>
       <c r="B15" s="0" t="n">
@@ -4140,7 +4136,7 @@
       <c r="M15" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="N15" s="50" t="n">
+      <c r="N15" s="49" t="n">
         <v>0.91317222078567</v>
       </c>
       <c r="O15" s="0" t="n">
@@ -4154,13 +4150,13 @@
       <c r="A16" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="B16" s="50" t="n">
+      <c r="B16" s="49" t="n">
         <v>0.39</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>0.25</v>
       </c>
-      <c r="D16" s="50" t="n">
+      <c r="D16" s="49" t="n">
         <v>9436</v>
       </c>
       <c r="E16" s="0" t="n">
@@ -4190,10 +4186,10 @@
       <c r="N16" s="0" t="n">
         <v>0.913048651839919</v>
       </c>
-      <c r="O16" s="50" t="n">
+      <c r="O16" s="49" t="n">
         <v>0.90435711446741</v>
       </c>
-      <c r="P16" s="34" t="n">
+      <c r="P16" s="1" t="n">
         <v>0.859851670962783</v>
       </c>
     </row>
@@ -4201,7 +4197,7 @@
       <c r="A17" s="0" t="s">
         <v>168</v>
       </c>
-      <c r="B17" s="50" t="n">
+      <c r="B17" s="49" t="n">
         <v>0.39</v>
       </c>
       <c r="C17" s="0" t="n">
@@ -4213,10 +4209,10 @@
       <c r="E17" s="0" t="n">
         <v>7140</v>
       </c>
-      <c r="F17" s="50" t="n">
+      <c r="F17" s="49" t="n">
         <v>132</v>
       </c>
-      <c r="G17" s="50" t="n">
+      <c r="G17" s="49" t="n">
         <v>65</v>
       </c>
       <c r="H17" s="0" t="n">
@@ -4280,22 +4276,22 @@
       <c r="A21" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="B21" s="50" t="n">
+      <c r="B21" s="49" t="n">
         <v>0.47</v>
       </c>
-      <c r="C21" s="50" t="n">
+      <c r="C21" s="49" t="n">
         <v>0.26</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>4163</v>
       </c>
-      <c r="E21" s="50" t="n">
+      <c r="E21" s="49" t="n">
         <v>1655</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="G21" s="50" t="n">
+      <c r="G21" s="49" t="n">
         <v>35</v>
       </c>
       <c r="H21" s="0" t="n">
@@ -4313,7 +4309,7 @@
       <c r="M21" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="N21" s="49" t="n">
+      <c r="N21" s="48" t="n">
         <v>0.936949630151462</v>
       </c>
       <c r="O21" s="0" t="n">
@@ -4324,22 +4320,22 @@
       <c r="A22" s="0" t="s">
         <v>170</v>
       </c>
-      <c r="B22" s="49" t="n">
+      <c r="B22" s="48" t="n">
         <v>0.48</v>
       </c>
-      <c r="C22" s="49" t="n">
+      <c r="C22" s="48" t="n">
         <v>0.29</v>
       </c>
-      <c r="D22" s="49" t="n">
+      <c r="D22" s="48" t="n">
         <v>4132</v>
       </c>
-      <c r="E22" s="49" t="n">
+      <c r="E22" s="48" t="n">
         <v>1645</v>
       </c>
-      <c r="F22" s="49" t="n">
+      <c r="F22" s="48" t="n">
         <v>71</v>
       </c>
-      <c r="G22" s="49" t="n">
+      <c r="G22" s="48" t="n">
         <v>60</v>
       </c>
       <c r="H22" s="0" t="n">
@@ -4360,7 +4356,7 @@
       <c r="N22" s="0" t="n">
         <v>0.935329341317367</v>
       </c>
-      <c r="O22" s="49" t="n">
+      <c r="O22" s="48" t="n">
         <v>0.931985380708409</v>
       </c>
     </row>
@@ -4409,10 +4405,10 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="49" t="s">
+      <c r="A24" s="48" t="s">
         <v>172</v>
       </c>
-      <c r="B24" s="50" t="n">
+      <c r="B24" s="49" t="n">
         <v>0.47</v>
       </c>
       <c r="C24" s="0" t="n">
@@ -4445,7 +4441,7 @@
       <c r="M24" s="0" t="s">
         <v>172</v>
       </c>
-      <c r="N24" s="50" t="n">
+      <c r="N24" s="49" t="n">
         <v>0.935166431842199</v>
       </c>
       <c r="O24" s="0" t="n">
@@ -4456,7 +4452,7 @@
       <c r="A25" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="B25" s="50" t="n">
+      <c r="B25" s="49" t="n">
         <v>0.47</v>
       </c>
       <c r="C25" s="0" t="n">
@@ -4500,7 +4496,7 @@
       <c r="A26" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="B26" s="50" t="n">
+      <c r="B26" s="49" t="n">
         <v>0.47</v>
       </c>
       <c r="C26" s="0" t="n">
@@ -4512,7 +4508,7 @@
       <c r="E26" s="0" t="n">
         <v>1694</v>
       </c>
-      <c r="F26" s="50" t="n">
+      <c r="F26" s="49" t="n">
         <v>60</v>
       </c>
       <c r="G26" s="0" t="n">
@@ -4536,7 +4532,7 @@
       <c r="N26" s="0" t="n">
         <v>0.933920394505108</v>
       </c>
-      <c r="O26" s="50" t="n">
+      <c r="O26" s="49" t="n">
         <v>0.928011903805282</v>
       </c>
     </row>
@@ -4591,13 +4587,13 @@
       <c r="B30" s="0" t="n">
         <v>0.36</v>
       </c>
-      <c r="C30" s="50" t="n">
+      <c r="C30" s="49" t="n">
         <v>0.16</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>6237</v>
       </c>
-      <c r="E30" s="49" t="n">
+      <c r="E30" s="48" t="n">
         <v>5566</v>
       </c>
       <c r="F30" s="0" t="n">
@@ -4632,22 +4628,22 @@
       <c r="A31" s="0" t="s">
         <v>176</v>
       </c>
-      <c r="B31" s="49" t="n">
+      <c r="B31" s="48" t="n">
         <v>0.42</v>
       </c>
-      <c r="C31" s="49" t="n">
+      <c r="C31" s="48" t="n">
         <v>0.18</v>
       </c>
-      <c r="D31" s="49" t="n">
+      <c r="D31" s="48" t="n">
         <v>5782</v>
       </c>
-      <c r="E31" s="50" t="n">
+      <c r="E31" s="49" t="n">
         <v>5570</v>
       </c>
-      <c r="F31" s="49" t="n">
+      <c r="F31" s="48" t="n">
         <v>123</v>
       </c>
-      <c r="G31" s="49" t="n">
+      <c r="G31" s="48" t="n">
         <v>53</v>
       </c>
       <c r="H31" s="0" t="n">
@@ -4665,10 +4661,10 @@
       <c r="M31" s="0" t="s">
         <v>176</v>
       </c>
-      <c r="N31" s="49" t="n">
+      <c r="N31" s="48" t="n">
         <v>0.86477807250221</v>
       </c>
-      <c r="O31" s="49" t="n">
+      <c r="O31" s="48" t="n">
         <v>0.939771112431267</v>
       </c>
     </row>
@@ -4717,16 +4713,16 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="49" t="s">
+      <c r="A33" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="B33" s="50" t="n">
+      <c r="B33" s="49" t="n">
         <v>0.41</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>0.15</v>
       </c>
-      <c r="D33" s="50" t="n">
+      <c r="D33" s="49" t="n">
         <v>5806</v>
       </c>
       <c r="E33" s="0" t="n">
@@ -4770,7 +4766,7 @@
       <c r="C34" s="0" t="n">
         <v>0.14</v>
       </c>
-      <c r="D34" s="34" t="n">
+      <c r="D34" s="1" t="n">
         <v>5844</v>
       </c>
       <c r="E34" s="0" t="n">
@@ -4808,7 +4804,7 @@
       <c r="A35" s="0" t="s">
         <v>180</v>
       </c>
-      <c r="B35" s="50" t="n">
+      <c r="B35" s="49" t="n">
         <v>0.41</v>
       </c>
       <c r="C35" s="0" t="n">
@@ -4820,10 +4816,10 @@
       <c r="E35" s="0" t="n">
         <v>5603</v>
       </c>
-      <c r="F35" s="50" t="n">
+      <c r="F35" s="49" t="n">
         <v>79</v>
       </c>
-      <c r="G35" s="50" t="n">
+      <c r="G35" s="49" t="n">
         <v>26</v>
       </c>
       <c r="H35" s="0" t="n">
@@ -4841,10 +4837,10 @@
       <c r="M35" s="0" t="s">
         <v>180</v>
       </c>
-      <c r="N35" s="50" t="n">
+      <c r="N35" s="49" t="n">
         <v>0.858079575596817</v>
       </c>
-      <c r="O35" s="50" t="n">
+      <c r="O35" s="49" t="n">
         <v>0.934191552672142</v>
       </c>
     </row>
@@ -4871,20 +4867,20 @@
   </sheetPr>
   <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S19" activeCellId="0" sqref="S19:S24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="9.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="30.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="30.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.41"/>
   </cols>
   <sheetData>

</xml_diff>